<commit_message>
8th commit : 1st test, ui good
</commit_message>
<xml_diff>
--- a/211005_Program_Test_List.xlsx
+++ b/211005_Program_Test_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijung\PycharmProjects\Load_Spectrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C32A92-07BE-471B-8135-FF35BB3EDBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598BF1C0-B39C-4DE4-B816-07B35DDD5EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E7DC293-06B9-4482-AE16-573205B167CF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
   <si>
     <t>Local To EQP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,10 +120,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>다운 중지 가능 유무</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>정상</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -132,19 +128,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>o</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>복합 폴더 파일2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>수정완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>확인중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확장자 선택 안했을 때</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확장자 all 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15min timeout test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EQP To Local</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -277,7 +281,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -302,13 +306,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,17 +336,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F725365D-EC05-4B91-B0EA-42513374B272}">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -671,74 +669,47 @@
     <row r="2" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="14" t="s">
+      <c r="C2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
+      <c r="C3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="V3" s="13"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -777,36 +748,6 @@
       <c r="L4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
@@ -815,30 +756,16 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="4"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -857,100 +784,42 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="4"/>
-    </row>
-    <row r="7" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="17" t="s">
+    </row>
+    <row r="7" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="20"/>
-    </row>
-    <row r="8" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="20"/>
+      <c r="B8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
@@ -969,16 +838,6 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="4"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -997,16 +856,6 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="4"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
@@ -1025,16 +874,6 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="4"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -1053,16 +892,6 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="4"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
@@ -1081,16 +910,6 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="4"/>
     </row>
     <row r="14" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
@@ -1109,30 +928,450 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="7"/>
+    </row>
+    <row r="15" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="17"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="14"/>
+      <c r="M17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="V17" s="14"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="4"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="4"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="11"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="11"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="4"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="4"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="4"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="4"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="4"/>
+    </row>
+    <row r="28" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="18">
+    <mergeCell ref="R16:V16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="U3:V3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>